<commit_message>
fix: upload reten baru updated tip top
</commit_message>
<xml_diff>
--- a/public/exports/MASA.xlsx
+++ b/public/exports/MASA.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t>Lampiran 2</t>
   </si>
@@ -29,10 +29,22 @@
     <t xml:space="preserve">NEGERI:    </t>
   </si>
   <si>
+    <t>Gi-Ret 2.0 (&lt;v2.0.10&gt;)</t>
+  </si>
+  <si>
     <t>DAERAH:</t>
   </si>
   <si>
+    <t>Maklumat dari &lt;Tarikh Mula&gt; - &lt;Tarikh Akhir&gt;</t>
+  </si>
+  <si>
     <t>FASILITI:</t>
+  </si>
+  <si>
+    <t>Peratus reten dilaporkan salah =  &lt;bilangan pesakit dengan reten salah/bilangan pesakit di reten*100&gt;%</t>
+  </si>
+  <si>
+    <t>Dijana oleh: &lt;Nama Penjana&gt; (&lt;Tarikh dan masa dijana&gt;)</t>
   </si>
   <si>
     <t>Maklumat berkenaan pesakit dipanggil untuk perkhidmatan kesihatan pergigian dalam tempoh 30 minit (Piagam Pelanggan Teras KKM)</t>
@@ -155,7 +167,7 @@
     <t xml:space="preserve">Jumlah pesakit yang dipanggil untuk perkhidmatan kesihatan pergigian dalam tempoh 30 minit  </t>
   </si>
   <si>
-    <t>Peratusan reten yang ditandakan salah</t>
+    <t>Catatan</t>
   </si>
   <si>
     <t xml:space="preserve">Jan </t>
@@ -207,36 +219,6 @@
   </si>
   <si>
     <t>Lampiran 2 - Maklumat Tambahan Piagam Pelanggan Teras KKM PKP Tahun 2023</t>
-  </si>
-  <si>
-    <t>Gi-Ret 2.0</t>
-  </si>
-  <si>
-    <t>v.2.0.8</t>
-  </si>
-  <si>
-    <t>Memaparkan maklumat dari</t>
-  </si>
-  <si>
-    <t>TARIKH MULA - TARIKH AKHIR</t>
-  </si>
-  <si>
-    <t>Tarikh dan masa penjanaan</t>
-  </si>
-  <si>
-    <t>TARIKH DAN MASA</t>
-  </si>
-  <si>
-    <t>Peratus reten dilaporkan salah</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> %</t>
-  </si>
-  <si>
-    <t>Dijana oleh</t>
-  </si>
-  <si>
-    <t>NAMA PENJANA (PERANAN)</t>
   </si>
 </sst>
 </file>
@@ -323,7 +305,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border/>
     <border>
       <bottom style="thin">
@@ -367,6 +349,11 @@
       <bottom/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
@@ -397,7 +384,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="47">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -418,10 +405,16 @@
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" shrinkToFit="0" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" shrinkToFit="0" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" vertical="center"/>
@@ -455,35 +448,39 @@
     <xf borderId="5" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="6" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="6" fillId="2" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="7" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="6" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="7" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="6" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="7" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="6" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="7" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="6" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="7" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="6" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="7" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="6" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="6" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="7" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="7" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="6" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="7" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="7" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="8" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="8" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="9" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="2" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -494,7 +491,7 @@
       <alignment horizontal="right" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
+      <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
@@ -736,7 +733,8 @@
     <col customWidth="1" min="6" max="6" width="30.14"/>
     <col customWidth="1" min="7" max="7" width="28.14"/>
     <col customWidth="1" min="8" max="8" width="22.29"/>
-    <col customWidth="1" min="9" max="16" width="8.86"/>
+    <col customWidth="1" min="9" max="9" width="18.43"/>
+    <col customWidth="1" min="10" max="16" width="8.86"/>
     <col customWidth="1" min="17" max="26" width="8.71"/>
   </cols>
   <sheetData>
@@ -794,15 +792,17 @@
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="8"/>
-      <c r="M3" s="8"/>
-      <c r="N3" s="8"/>
-      <c r="O3" s="8"/>
-      <c r="P3" s="8"/>
+      <c r="H3" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="I3" s="8"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="9"/>
+      <c r="M3" s="9"/>
+      <c r="N3" s="9"/>
+      <c r="O3" s="9"/>
+      <c r="P3" s="9"/>
       <c r="Q3" s="2"/>
       <c r="R3" s="2"/>
       <c r="S3" s="2"/>
@@ -816,21 +816,23 @@
     </row>
     <row r="4">
       <c r="A4" s="6" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B4" s="6"/>
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="7"/>
-      <c r="J4" s="8"/>
-      <c r="K4" s="8"/>
-      <c r="L4" s="8"/>
-      <c r="M4" s="8"/>
-      <c r="N4" s="8"/>
-      <c r="O4" s="8"/>
-      <c r="P4" s="8"/>
+      <c r="H4" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="I4" s="8"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="9"/>
+      <c r="M4" s="9"/>
+      <c r="N4" s="9"/>
+      <c r="O4" s="9"/>
+      <c r="P4" s="9"/>
       <c r="Q4" s="2"/>
       <c r="R4" s="2"/>
       <c r="S4" s="2"/>
@@ -844,21 +846,23 @@
     </row>
     <row r="5">
       <c r="A5" s="6" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B5" s="6"/>
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
       <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="7"/>
-      <c r="J5" s="8"/>
-      <c r="K5" s="8"/>
-      <c r="L5" s="8"/>
-      <c r="M5" s="8"/>
-      <c r="N5" s="8"/>
-      <c r="O5" s="8"/>
-      <c r="P5" s="8"/>
+      <c r="H5" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="I5" s="8"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="9"/>
+      <c r="M5" s="9"/>
+      <c r="N5" s="9"/>
+      <c r="O5" s="9"/>
+      <c r="P5" s="9"/>
       <c r="Q5" s="2"/>
       <c r="R5" s="2"/>
       <c r="S5" s="2"/>
@@ -878,15 +882,17 @@
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="8"/>
-      <c r="K6" s="8"/>
-      <c r="L6" s="8"/>
-      <c r="M6" s="8"/>
-      <c r="N6" s="8"/>
-      <c r="O6" s="8"/>
-      <c r="P6" s="8"/>
+      <c r="H6" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="I6" s="8"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="9"/>
+      <c r="M6" s="9"/>
+      <c r="N6" s="9"/>
+      <c r="O6" s="9"/>
+      <c r="P6" s="9"/>
       <c r="Q6" s="2"/>
       <c r="R6" s="2"/>
       <c r="S6" s="2"/>
@@ -899,17 +905,17 @@
       <c r="Z6" s="2"/>
     </row>
     <row r="7">
-      <c r="A7" s="9" t="s">
-        <v>5</v>
+      <c r="A7" s="11" t="s">
+        <v>9</v>
       </c>
-      <c r="I7" s="10"/>
-      <c r="J7" s="10"/>
-      <c r="K7" s="10"/>
-      <c r="L7" s="11"/>
-      <c r="M7" s="11"/>
-      <c r="N7" s="11"/>
-      <c r="O7" s="11"/>
-      <c r="P7" s="11"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="12"/>
+      <c r="K7" s="12"/>
+      <c r="L7" s="13"/>
+      <c r="M7" s="13"/>
+      <c r="N7" s="13"/>
+      <c r="O7" s="13"/>
+      <c r="P7" s="13"/>
       <c r="Q7" s="2"/>
       <c r="R7" s="2"/>
       <c r="S7" s="2"/>
@@ -922,16 +928,16 @@
       <c r="Z7" s="2"/>
     </row>
     <row r="8">
-      <c r="A8" s="12" t="s">
-        <v>6</v>
+      <c r="A8" s="14" t="s">
+        <v>10</v>
       </c>
-      <c r="B8" s="13"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="13"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
@@ -952,187 +958,187 @@
       <c r="Z8" s="2"/>
     </row>
     <row r="9" ht="33.75" customHeight="1">
-      <c r="A9" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="15"/>
-      <c r="C9" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" s="17"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="17"/>
-      <c r="G9" s="17"/>
-      <c r="H9" s="15"/>
-      <c r="I9" s="18"/>
-      <c r="J9" s="18"/>
-      <c r="K9" s="18"/>
-      <c r="L9" s="18"/>
-      <c r="M9" s="19"/>
-      <c r="N9" s="19"/>
-      <c r="O9" s="19"/>
-      <c r="P9" s="19"/>
-      <c r="Q9" s="19"/>
-      <c r="R9" s="19"/>
-      <c r="S9" s="19"/>
-      <c r="T9" s="19"/>
-      <c r="U9" s="19"/>
-      <c r="V9" s="19"/>
-      <c r="W9" s="19"/>
-      <c r="X9" s="19"/>
-      <c r="Y9" s="19"/>
-      <c r="Z9" s="19"/>
-    </row>
-    <row r="10" ht="33.0" customHeight="1">
-      <c r="A10" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="15"/>
-      <c r="C10" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="17"/>
-      <c r="H10" s="15"/>
-      <c r="I10" s="18"/>
-      <c r="J10" s="18"/>
-      <c r="K10" s="18"/>
-      <c r="L10" s="18"/>
-      <c r="M10" s="19"/>
-      <c r="N10" s="19"/>
-      <c r="O10" s="19"/>
-      <c r="P10" s="19"/>
-      <c r="Q10" s="19"/>
-      <c r="R10" s="19"/>
-      <c r="S10" s="19"/>
-      <c r="T10" s="19"/>
-      <c r="U10" s="19"/>
-      <c r="V10" s="19"/>
-      <c r="W10" s="19"/>
-      <c r="X10" s="19"/>
-      <c r="Y10" s="19"/>
-      <c r="Z10" s="19"/>
-    </row>
-    <row r="11" ht="30.75" customHeight="1">
-      <c r="A11" s="21" t="s">
+      <c r="A9" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="15"/>
-      <c r="C11" s="16" t="s">
+      <c r="B9" s="17"/>
+      <c r="C9" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="17"/>
-      <c r="G11" s="17"/>
-      <c r="H11" s="15"/>
-      <c r="I11" s="18"/>
-      <c r="J11" s="18"/>
-      <c r="K11" s="18"/>
-      <c r="L11" s="18"/>
-      <c r="M11" s="19"/>
-      <c r="N11" s="19"/>
-      <c r="O11" s="19"/>
-      <c r="P11" s="19"/>
-      <c r="Q11" s="19"/>
-      <c r="R11" s="19"/>
-      <c r="S11" s="19"/>
-      <c r="T11" s="19"/>
-      <c r="U11" s="19"/>
-      <c r="V11" s="19"/>
-      <c r="W11" s="19"/>
-      <c r="X11" s="19"/>
-      <c r="Y11" s="19"/>
-      <c r="Z11" s="19"/>
-    </row>
-    <row r="12" ht="30.75" customHeight="1">
-      <c r="A12" s="14" t="s">
+      <c r="D9" s="19"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="19"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="20"/>
+      <c r="J9" s="20"/>
+      <c r="K9" s="20"/>
+      <c r="L9" s="20"/>
+      <c r="M9" s="21"/>
+      <c r="N9" s="21"/>
+      <c r="O9" s="21"/>
+      <c r="P9" s="21"/>
+      <c r="Q9" s="21"/>
+      <c r="R9" s="21"/>
+      <c r="S9" s="21"/>
+      <c r="T9" s="21"/>
+      <c r="U9" s="21"/>
+      <c r="V9" s="21"/>
+      <c r="W9" s="21"/>
+      <c r="X9" s="21"/>
+      <c r="Y9" s="21"/>
+      <c r="Z9" s="21"/>
+    </row>
+    <row r="10" ht="33.0" customHeight="1">
+      <c r="A10" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="15"/>
-      <c r="C12" s="16" t="s">
+      <c r="B10" s="17"/>
+      <c r="C10" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="17"/>
-      <c r="G12" s="17"/>
-      <c r="H12" s="15"/>
-      <c r="I12" s="18"/>
-      <c r="J12" s="18"/>
-      <c r="K12" s="18"/>
-      <c r="L12" s="18"/>
-      <c r="M12" s="19"/>
-      <c r="N12" s="19"/>
-      <c r="O12" s="19"/>
-      <c r="P12" s="19"/>
-      <c r="Q12" s="19"/>
-      <c r="R12" s="19"/>
-      <c r="S12" s="19"/>
-      <c r="T12" s="19"/>
-      <c r="U12" s="19"/>
-      <c r="V12" s="19"/>
-      <c r="W12" s="19"/>
-      <c r="X12" s="19"/>
-      <c r="Y12" s="19"/>
-      <c r="Z12" s="19"/>
-    </row>
-    <row r="13" ht="30.75" customHeight="1">
-      <c r="A13" s="22"/>
-      <c r="B13" s="22"/>
-      <c r="C13" s="22"/>
-      <c r="D13" s="22"/>
-      <c r="E13" s="22"/>
-      <c r="F13" s="22"/>
-      <c r="G13" s="19"/>
-      <c r="H13" s="19"/>
-      <c r="I13" s="19"/>
-      <c r="J13" s="19"/>
-      <c r="K13" s="19"/>
-      <c r="L13" s="19"/>
-      <c r="M13" s="19"/>
-      <c r="N13" s="19"/>
-      <c r="O13" s="19"/>
-      <c r="P13" s="19"/>
-      <c r="Q13" s="19"/>
-      <c r="R13" s="19"/>
-      <c r="S13" s="19"/>
-      <c r="T13" s="19"/>
-      <c r="U13" s="19"/>
-      <c r="V13" s="19"/>
-      <c r="W13" s="19"/>
-      <c r="X13" s="19"/>
-      <c r="Y13" s="19"/>
-      <c r="Z13" s="19"/>
-    </row>
-    <row r="14" ht="87.0" customHeight="1">
-      <c r="A14" s="23" t="s">
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="20"/>
+      <c r="J10" s="20"/>
+      <c r="K10" s="20"/>
+      <c r="L10" s="20"/>
+      <c r="M10" s="21"/>
+      <c r="N10" s="21"/>
+      <c r="O10" s="21"/>
+      <c r="P10" s="21"/>
+      <c r="Q10" s="21"/>
+      <c r="R10" s="21"/>
+      <c r="S10" s="21"/>
+      <c r="T10" s="21"/>
+      <c r="U10" s="21"/>
+      <c r="V10" s="21"/>
+      <c r="W10" s="21"/>
+      <c r="X10" s="21"/>
+      <c r="Y10" s="21"/>
+      <c r="Z10" s="21"/>
+    </row>
+    <row r="11" ht="30.75" customHeight="1">
+      <c r="A11" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="23" t="s">
+      <c r="B11" s="17"/>
+      <c r="C11" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="C14" s="23" t="s">
+      <c r="D11" s="19"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="19"/>
+      <c r="H11" s="17"/>
+      <c r="I11" s="20"/>
+      <c r="J11" s="20"/>
+      <c r="K11" s="20"/>
+      <c r="L11" s="20"/>
+      <c r="M11" s="21"/>
+      <c r="N11" s="21"/>
+      <c r="O11" s="21"/>
+      <c r="P11" s="21"/>
+      <c r="Q11" s="21"/>
+      <c r="R11" s="21"/>
+      <c r="S11" s="21"/>
+      <c r="T11" s="21"/>
+      <c r="U11" s="21"/>
+      <c r="V11" s="21"/>
+      <c r="W11" s="21"/>
+      <c r="X11" s="21"/>
+      <c r="Y11" s="21"/>
+      <c r="Z11" s="21"/>
+    </row>
+    <row r="12" ht="30.75" customHeight="1">
+      <c r="A12" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="D14" s="24" t="s">
+      <c r="B12" s="17"/>
+      <c r="C12" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="E14" s="23" t="s">
+      <c r="D12" s="19"/>
+      <c r="E12" s="19"/>
+      <c r="F12" s="19"/>
+      <c r="G12" s="19"/>
+      <c r="H12" s="17"/>
+      <c r="I12" s="20"/>
+      <c r="J12" s="20"/>
+      <c r="K12" s="20"/>
+      <c r="L12" s="20"/>
+      <c r="M12" s="21"/>
+      <c r="N12" s="21"/>
+      <c r="O12" s="21"/>
+      <c r="P12" s="21"/>
+      <c r="Q12" s="21"/>
+      <c r="R12" s="21"/>
+      <c r="S12" s="21"/>
+      <c r="T12" s="21"/>
+      <c r="U12" s="21"/>
+      <c r="V12" s="21"/>
+      <c r="W12" s="21"/>
+      <c r="X12" s="21"/>
+      <c r="Y12" s="21"/>
+      <c r="Z12" s="21"/>
+    </row>
+    <row r="13" ht="30.75" customHeight="1">
+      <c r="A13" s="24"/>
+      <c r="B13" s="24"/>
+      <c r="C13" s="24"/>
+      <c r="D13" s="24"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="24"/>
+      <c r="G13" s="21"/>
+      <c r="H13" s="25"/>
+      <c r="I13" s="25"/>
+      <c r="J13" s="21"/>
+      <c r="K13" s="21"/>
+      <c r="L13" s="21"/>
+      <c r="M13" s="21"/>
+      <c r="N13" s="21"/>
+      <c r="O13" s="21"/>
+      <c r="P13" s="21"/>
+      <c r="Q13" s="21"/>
+      <c r="R13" s="21"/>
+      <c r="S13" s="21"/>
+      <c r="T13" s="21"/>
+      <c r="U13" s="21"/>
+      <c r="V13" s="21"/>
+      <c r="W13" s="21"/>
+      <c r="X13" s="21"/>
+      <c r="Y13" s="21"/>
+      <c r="Z13" s="21"/>
+    </row>
+    <row r="14" ht="87.0" customHeight="1">
+      <c r="A14" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="F14" s="23" t="s">
+      <c r="B14" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="G14" s="25" t="s">
+      <c r="C14" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="H14" s="26" t="s">
+      <c r="D14" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="I14" s="2"/>
+      <c r="E14" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="F14" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="G14" s="28" t="s">
+        <v>25</v>
+      </c>
+      <c r="H14" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="I14" s="30"/>
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
@@ -1152,22 +1158,22 @@
       <c r="Z14" s="2"/>
     </row>
     <row r="15" ht="19.5" customHeight="1">
-      <c r="A15" s="27" t="s">
-        <v>23</v>
+      <c r="A15" s="31" t="s">
+        <v>27</v>
       </c>
-      <c r="B15" s="27"/>
-      <c r="C15" s="27"/>
-      <c r="D15" s="27">
+      <c r="B15" s="31"/>
+      <c r="C15" s="31"/>
+      <c r="D15" s="31">
         <f t="shared" ref="D15:D20" si="1">SUM(B15+C15)</f>
         <v>0</v>
       </c>
-      <c r="E15" s="28"/>
-      <c r="F15" s="28"/>
-      <c r="G15" s="27">
+      <c r="E15" s="32"/>
+      <c r="F15" s="32"/>
+      <c r="G15" s="31">
         <f t="shared" ref="G15:G20" si="2">sum(E15:F15)</f>
         <v>0</v>
       </c>
-      <c r="H15" s="29"/>
+      <c r="H15" s="33"/>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
@@ -1188,22 +1194,22 @@
       <c r="Z15" s="2"/>
     </row>
     <row r="16" ht="19.5" customHeight="1">
-      <c r="A16" s="27" t="s">
-        <v>24</v>
+      <c r="A16" s="31" t="s">
+        <v>28</v>
       </c>
-      <c r="B16" s="27"/>
-      <c r="C16" s="27"/>
-      <c r="D16" s="27">
+      <c r="B16" s="31"/>
+      <c r="C16" s="31"/>
+      <c r="D16" s="31">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E16" s="28"/>
-      <c r="F16" s="28"/>
-      <c r="G16" s="27">
+      <c r="E16" s="32"/>
+      <c r="F16" s="32"/>
+      <c r="G16" s="31">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="H16" s="29"/>
+      <c r="H16" s="33"/>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
@@ -1224,22 +1230,22 @@
       <c r="Z16" s="2"/>
     </row>
     <row r="17" ht="19.5" customHeight="1">
-      <c r="A17" s="27" t="s">
-        <v>25</v>
+      <c r="A17" s="31" t="s">
+        <v>29</v>
       </c>
-      <c r="B17" s="27"/>
-      <c r="C17" s="27"/>
-      <c r="D17" s="27">
+      <c r="B17" s="31"/>
+      <c r="C17" s="31"/>
+      <c r="D17" s="31">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E17" s="28"/>
-      <c r="F17" s="28"/>
-      <c r="G17" s="27">
+      <c r="E17" s="32"/>
+      <c r="F17" s="32"/>
+      <c r="G17" s="31">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="H17" s="29"/>
+      <c r="H17" s="33"/>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
@@ -1260,22 +1266,22 @@
       <c r="Z17" s="2"/>
     </row>
     <row r="18" ht="19.5" customHeight="1">
-      <c r="A18" s="27" t="s">
-        <v>26</v>
+      <c r="A18" s="31" t="s">
+        <v>30</v>
       </c>
-      <c r="B18" s="27"/>
-      <c r="C18" s="27"/>
-      <c r="D18" s="27">
+      <c r="B18" s="31"/>
+      <c r="C18" s="31"/>
+      <c r="D18" s="31">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E18" s="28"/>
-      <c r="F18" s="28"/>
-      <c r="G18" s="27">
+      <c r="E18" s="32"/>
+      <c r="F18" s="32"/>
+      <c r="G18" s="31">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="H18" s="29"/>
+      <c r="H18" s="33"/>
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
@@ -1296,22 +1302,22 @@
       <c r="Z18" s="2"/>
     </row>
     <row r="19" ht="19.5" customHeight="1">
-      <c r="A19" s="27" t="s">
-        <v>27</v>
+      <c r="A19" s="31" t="s">
+        <v>31</v>
       </c>
-      <c r="B19" s="27"/>
-      <c r="C19" s="27"/>
-      <c r="D19" s="27">
+      <c r="B19" s="31"/>
+      <c r="C19" s="31"/>
+      <c r="D19" s="31">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E19" s="28"/>
-      <c r="F19" s="28"/>
-      <c r="G19" s="27">
+      <c r="E19" s="32"/>
+      <c r="F19" s="32"/>
+      <c r="G19" s="31">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="H19" s="29"/>
+      <c r="H19" s="33"/>
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
@@ -1332,22 +1338,22 @@
       <c r="Z19" s="2"/>
     </row>
     <row r="20" ht="19.5" customHeight="1">
-      <c r="A20" s="27" t="s">
-        <v>28</v>
+      <c r="A20" s="31" t="s">
+        <v>32</v>
       </c>
-      <c r="B20" s="27"/>
-      <c r="C20" s="27"/>
-      <c r="D20" s="27">
+      <c r="B20" s="31"/>
+      <c r="C20" s="31"/>
+      <c r="D20" s="31">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E20" s="28"/>
-      <c r="F20" s="28"/>
-      <c r="G20" s="27">
+      <c r="E20" s="32"/>
+      <c r="F20" s="32"/>
+      <c r="G20" s="31">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="H20" s="29"/>
+      <c r="H20" s="33"/>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
       <c r="K20" s="2"/>
@@ -1368,34 +1374,34 @@
       <c r="Z20" s="2"/>
     </row>
     <row r="21" ht="19.5" customHeight="1">
-      <c r="A21" s="23" t="s">
-        <v>29</v>
+      <c r="A21" s="26" t="s">
+        <v>33</v>
       </c>
-      <c r="B21" s="27">
+      <c r="B21" s="31">
         <f t="shared" ref="B21:G21" si="3">SUM(B15:B20)</f>
         <v>0</v>
       </c>
-      <c r="C21" s="27">
+      <c r="C21" s="31">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="D21" s="30">
+      <c r="D21" s="34">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="E21" s="28">
+      <c r="E21" s="32">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="F21" s="28">
+      <c r="F21" s="32">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="G21" s="31">
+      <c r="G21" s="35">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="H21" s="29"/>
+      <c r="H21" s="33"/>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
       <c r="K21" s="2"/>
@@ -1416,22 +1422,22 @@
       <c r="Z21" s="2"/>
     </row>
     <row r="22" ht="19.5" customHeight="1">
-      <c r="A22" s="27" t="s">
-        <v>30</v>
+      <c r="A22" s="31" t="s">
+        <v>34</v>
       </c>
-      <c r="B22" s="27"/>
-      <c r="C22" s="27"/>
-      <c r="D22" s="27">
+      <c r="B22" s="31"/>
+      <c r="C22" s="31"/>
+      <c r="D22" s="31">
         <f t="shared" ref="D22:D27" si="4">SUM(B22+C22)</f>
         <v>0</v>
       </c>
-      <c r="E22" s="28"/>
-      <c r="F22" s="28"/>
-      <c r="G22" s="27">
+      <c r="E22" s="32"/>
+      <c r="F22" s="32"/>
+      <c r="G22" s="31">
         <f t="shared" ref="G22:G27" si="5">sum(E22:F22)</f>
         <v>0</v>
       </c>
-      <c r="H22" s="29"/>
+      <c r="H22" s="33"/>
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
@@ -1452,22 +1458,22 @@
       <c r="Z22" s="2"/>
     </row>
     <row r="23" ht="19.5" customHeight="1">
-      <c r="A23" s="27" t="s">
-        <v>31</v>
+      <c r="A23" s="31" t="s">
+        <v>35</v>
       </c>
-      <c r="B23" s="27"/>
-      <c r="C23" s="27"/>
-      <c r="D23" s="27">
+      <c r="B23" s="31"/>
+      <c r="C23" s="31"/>
+      <c r="D23" s="31">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="E23" s="28"/>
-      <c r="F23" s="28"/>
-      <c r="G23" s="27">
+      <c r="E23" s="32"/>
+      <c r="F23" s="32"/>
+      <c r="G23" s="31">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="H23" s="29"/>
+      <c r="H23" s="33"/>
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
       <c r="K23" s="2"/>
@@ -1488,22 +1494,22 @@
       <c r="Z23" s="2"/>
     </row>
     <row r="24" ht="19.5" customHeight="1">
-      <c r="A24" s="27" t="s">
-        <v>32</v>
+      <c r="A24" s="31" t="s">
+        <v>36</v>
       </c>
-      <c r="B24" s="27"/>
-      <c r="C24" s="27"/>
-      <c r="D24" s="27">
+      <c r="B24" s="31"/>
+      <c r="C24" s="31"/>
+      <c r="D24" s="31">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="E24" s="28"/>
-      <c r="F24" s="28"/>
-      <c r="G24" s="27">
+      <c r="E24" s="32"/>
+      <c r="F24" s="32"/>
+      <c r="G24" s="31">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="H24" s="29"/>
+      <c r="H24" s="33"/>
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
       <c r="K24" s="2"/>
@@ -1524,22 +1530,22 @@
       <c r="Z24" s="2"/>
     </row>
     <row r="25" ht="19.5" customHeight="1">
-      <c r="A25" s="27" t="s">
-        <v>33</v>
+      <c r="A25" s="31" t="s">
+        <v>37</v>
       </c>
-      <c r="B25" s="27"/>
-      <c r="C25" s="27"/>
-      <c r="D25" s="27">
+      <c r="B25" s="31"/>
+      <c r="C25" s="31"/>
+      <c r="D25" s="31">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="E25" s="28"/>
-      <c r="F25" s="28"/>
-      <c r="G25" s="27">
+      <c r="E25" s="32"/>
+      <c r="F25" s="32"/>
+      <c r="G25" s="31">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="H25" s="29"/>
+      <c r="H25" s="33"/>
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
       <c r="K25" s="2"/>
@@ -1560,22 +1566,22 @@
       <c r="Z25" s="2"/>
     </row>
     <row r="26" ht="19.5" customHeight="1">
-      <c r="A26" s="27" t="s">
-        <v>34</v>
+      <c r="A26" s="31" t="s">
+        <v>38</v>
       </c>
-      <c r="B26" s="27"/>
-      <c r="C26" s="27"/>
-      <c r="D26" s="27">
+      <c r="B26" s="31"/>
+      <c r="C26" s="31"/>
+      <c r="D26" s="31">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="E26" s="28"/>
-      <c r="F26" s="28"/>
-      <c r="G26" s="27">
+      <c r="E26" s="32"/>
+      <c r="F26" s="32"/>
+      <c r="G26" s="31">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="H26" s="29"/>
+      <c r="H26" s="33"/>
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
       <c r="K26" s="2"/>
@@ -1596,22 +1602,22 @@
       <c r="Z26" s="2"/>
     </row>
     <row r="27" ht="19.5" customHeight="1">
-      <c r="A27" s="27" t="s">
-        <v>35</v>
+      <c r="A27" s="31" t="s">
+        <v>39</v>
       </c>
-      <c r="B27" s="27"/>
-      <c r="C27" s="27"/>
-      <c r="D27" s="27">
+      <c r="B27" s="31"/>
+      <c r="C27" s="31"/>
+      <c r="D27" s="31">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="E27" s="28"/>
-      <c r="F27" s="28"/>
-      <c r="G27" s="27">
+      <c r="E27" s="32"/>
+      <c r="F27" s="32"/>
+      <c r="G27" s="31">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="H27" s="29"/>
+      <c r="H27" s="33"/>
       <c r="I27" s="2"/>
       <c r="J27" s="2"/>
       <c r="K27" s="2"/>
@@ -1632,34 +1638,34 @@
       <c r="Z27" s="2"/>
     </row>
     <row r="28" ht="19.5" customHeight="1">
-      <c r="A28" s="23" t="s">
-        <v>36</v>
+      <c r="A28" s="26" t="s">
+        <v>40</v>
       </c>
-      <c r="B28" s="27">
+      <c r="B28" s="31">
         <f t="shared" ref="B28:G28" si="6">SUM(B21:B27)</f>
         <v>0</v>
       </c>
-      <c r="C28" s="27">
+      <c r="C28" s="31">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="D28" s="30">
+      <c r="D28" s="34">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="E28" s="28">
+      <c r="E28" s="32">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="F28" s="28">
+      <c r="F28" s="32">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="G28" s="31">
+      <c r="G28" s="35">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="H28" s="29"/>
+      <c r="H28" s="33"/>
       <c r="I28" s="2"/>
       <c r="J28" s="2"/>
       <c r="K28" s="2"/>
@@ -1680,13 +1686,13 @@
       <c r="Z28" s="2"/>
     </row>
     <row r="29" ht="21.0" customHeight="1">
-      <c r="A29" s="32"/>
-      <c r="B29" s="33"/>
-      <c r="C29" s="33"/>
-      <c r="D29" s="33"/>
-      <c r="E29" s="33"/>
-      <c r="F29" s="33"/>
-      <c r="G29" s="33"/>
+      <c r="A29" s="36"/>
+      <c r="B29" s="37"/>
+      <c r="C29" s="37"/>
+      <c r="D29" s="37"/>
+      <c r="E29" s="37"/>
+      <c r="F29" s="37"/>
+      <c r="G29" s="37"/>
       <c r="H29" s="2"/>
       <c r="I29" s="2"/>
       <c r="J29" s="2"/>
@@ -1708,19 +1714,19 @@
       <c r="Z29" s="2"/>
     </row>
     <row r="30" ht="15.0" customHeight="1">
-      <c r="A30" s="34" t="s">
-        <v>37</v>
+      <c r="A30" s="38" t="s">
+        <v>41</v>
       </c>
-      <c r="B30" s="17"/>
-      <c r="C30" s="15"/>
-      <c r="D30" s="35" t="str">
+      <c r="B30" s="19"/>
+      <c r="C30" s="17"/>
+      <c r="D30" s="39" t="str">
         <f>G21/D21</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="E30" s="17"/>
-      <c r="F30" s="17"/>
-      <c r="G30" s="17"/>
-      <c r="H30" s="15"/>
+      <c r="E30" s="19"/>
+      <c r="F30" s="19"/>
+      <c r="G30" s="19"/>
+      <c r="H30" s="17"/>
       <c r="I30" s="2"/>
       <c r="J30" s="2"/>
       <c r="K30" s="2"/>
@@ -1741,19 +1747,19 @@
       <c r="Z30" s="2"/>
     </row>
     <row r="31" ht="15.0" customHeight="1">
-      <c r="A31" s="34" t="s">
-        <v>38</v>
+      <c r="A31" s="38" t="s">
+        <v>42</v>
       </c>
-      <c r="B31" s="17"/>
-      <c r="C31" s="15"/>
-      <c r="D31" s="35" t="str">
+      <c r="B31" s="19"/>
+      <c r="C31" s="17"/>
+      <c r="D31" s="39" t="str">
         <f>G28/D28</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="E31" s="17"/>
-      <c r="F31" s="17"/>
-      <c r="G31" s="17"/>
-      <c r="H31" s="15"/>
+      <c r="E31" s="19"/>
+      <c r="F31" s="19"/>
+      <c r="G31" s="19"/>
+      <c r="H31" s="17"/>
       <c r="I31" s="2"/>
       <c r="J31" s="2"/>
       <c r="K31" s="2"/>
@@ -1802,8 +1808,8 @@
       <c r="Z32" s="2"/>
     </row>
     <row r="33" ht="15.75" customHeight="1">
-      <c r="A33" s="36" t="s">
-        <v>39</v>
+      <c r="A33" s="40" t="s">
+        <v>43</v>
       </c>
       <c r="I33" s="2"/>
       <c r="J33" s="2"/>
@@ -1825,9 +1831,7 @@
       <c r="Z33" s="2"/>
     </row>
     <row r="34" ht="15.75" customHeight="1">
-      <c r="A34" s="37" t="s">
-        <v>40</v>
-      </c>
+      <c r="A34" s="41"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
@@ -1855,9 +1859,7 @@
       <c r="Z34" s="2"/>
     </row>
     <row r="35" ht="15.75" customHeight="1">
-      <c r="A35" s="38" t="s">
-        <v>41</v>
-      </c>
+      <c r="A35" s="42"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
@@ -1885,9 +1887,7 @@
       <c r="Z35" s="2"/>
     </row>
     <row r="36" ht="15.75" customHeight="1">
-      <c r="A36" s="39" t="s">
-        <v>42</v>
-      </c>
+      <c r="A36" s="43"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
@@ -1915,9 +1915,7 @@
       <c r="Z36" s="2"/>
     </row>
     <row r="37" ht="15.75" customHeight="1">
-      <c r="A37" s="40" t="s">
-        <v>43</v>
-      </c>
+      <c r="A37" s="44"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
@@ -1945,9 +1943,7 @@
       <c r="Z37" s="2"/>
     </row>
     <row r="38" ht="15.75" customHeight="1">
-      <c r="A38" s="39" t="s">
-        <v>44</v>
-      </c>
+      <c r="A38" s="43"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
@@ -1975,9 +1971,7 @@
       <c r="Z38" s="2"/>
     </row>
     <row r="39" ht="15.75" customHeight="1">
-      <c r="A39" s="38" t="s">
-        <v>45</v>
-      </c>
+      <c r="A39" s="42"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
@@ -2005,9 +1999,7 @@
       <c r="Z39" s="2"/>
     </row>
     <row r="40" ht="15.0" customHeight="1">
-      <c r="A40" s="41" t="s">
-        <v>46</v>
-      </c>
+      <c r="A40" s="45"/>
       <c r="I40" s="2"/>
       <c r="J40" s="2"/>
       <c r="K40" s="2"/>
@@ -2028,9 +2020,7 @@
       <c r="Z40" s="2"/>
     </row>
     <row r="41" ht="15.75" customHeight="1">
-      <c r="A41" s="38" t="s">
-        <v>47</v>
-      </c>
+      <c r="A41" s="42"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
@@ -2058,9 +2048,7 @@
       <c r="Z41" s="2"/>
     </row>
     <row r="42" ht="15.75" customHeight="1">
-      <c r="A42" s="42" t="s">
-        <v>48</v>
-      </c>
+      <c r="A42" s="46"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
@@ -2088,9 +2076,7 @@
       <c r="Z42" s="2"/>
     </row>
     <row r="43" ht="15.75" customHeight="1">
-      <c r="A43" s="40" t="s">
-        <v>49</v>
-      </c>
+      <c r="A43" s="44"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
@@ -28999,27 +28985,27 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="A7:H7"/>
+    <mergeCell ref="A8:H8"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A29:G29"/>
     <mergeCell ref="A30:C30"/>
     <mergeCell ref="D30:H30"/>
     <mergeCell ref="A31:C31"/>
     <mergeCell ref="D31:H31"/>
     <mergeCell ref="A33:H33"/>
+    <mergeCell ref="A9:B9"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="C10:H10"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="C11:H11"/>
-    <mergeCell ref="A12:B12"/>
     <mergeCell ref="C12:H12"/>
-    <mergeCell ref="A29:G29"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A2:H2"/>
-    <mergeCell ref="A7:H7"/>
-    <mergeCell ref="A8:H8"/>
-    <mergeCell ref="A9:B9"/>
     <mergeCell ref="C9:H9"/>
-    <mergeCell ref="B3:D3"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins bottom="0.15748031496062992" footer="0.0" header="0.0" left="0.1968503937007874" right="0.1968503937007874" top="0.35433070866141736"/>

</xml_diff>